<commit_message>
Task Interface und BackendService erstellt, in List-K. Backend eingebunden, auslesen des Taskarrays in Tabelle
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BC5F2E-2AB0-49AD-ABD2-66C4E6CD1760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70E89CF-0EDB-48CC-A34F-867EDA3CC6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="30.09." sheetId="2" r:id="rId2"/>
+    <sheet name="Notizen Präsi" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -171,6 +173,18 @@
   </si>
   <si>
     <t>dele one 30.09.</t>
+  </si>
+  <si>
+    <t>Backend starten</t>
+  </si>
+  <si>
+    <t>Frontend starten</t>
+  </si>
+  <si>
+    <t>interface und service im frontend angelegt+</t>
+  </si>
+  <si>
+    <t>klären === und == ?</t>
   </si>
 </sst>
 </file>
@@ -560,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -779,4 +793,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988DF169-2626-45E6-A36A-F4AD1A4B6C9F}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600CCC3B-98C2-4D2B-BFEA-D00A9F2B4598}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
in Liste nur offene Tasks anzeigen, filter funktioniert noch nicht
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70E89CF-0EDB-48CC-A34F-867EDA3CC6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6E0F11-A3EA-4147-85BB-DEFA3953F420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -181,10 +181,10 @@
     <t>Frontend starten</t>
   </si>
   <si>
-    <t>interface und service im frontend angelegt+</t>
-  </si>
-  <si>
     <t>klären === und == ?</t>
+  </si>
+  <si>
+    <t>Archivbutton</t>
   </si>
 </sst>
 </file>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -601,7 +601,7 @@
       <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F2" t="s">
@@ -635,21 +635,19 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
+      <c r="E7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -660,10 +658,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -673,6 +668,12 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -681,12 +682,6 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -695,8 +690,11 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -707,12 +705,12 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -720,31 +718,31 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>11</v>
       </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -752,11 +750,16 @@
         <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E22" t="s">
         <v>35</v>
       </c>
     </row>
@@ -797,20 +800,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988DF169-2626-45E6-A36A-F4AD1A4B6C9F}">
-  <dimension ref="A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -819,7 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600CCC3B-98C2-4D2B-BFEA-D00A9F2B4598}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -837,7 +834,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filter in List und Archiv funktioniert, Belegen der FormControlElemente in Update funktioniert nicht
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6E0F11-A3EA-4147-85BB-DEFA3953F420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9343F5-DC46-4D11-89AF-84C6A0D2F9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -185,6 +185,24 @@
   </si>
   <si>
     <t>Archivbutton</t>
+  </si>
+  <si>
+    <t>await war wegen promise?</t>
+  </si>
+  <si>
+    <t>filter in Liste und Archiv funktionieren</t>
+  </si>
+  <si>
+    <t>in Liste bearbeiten und delte button bearbeitet</t>
+  </si>
+  <si>
+    <t>reactive forms</t>
+  </si>
+  <si>
+    <t>activated route</t>
+  </si>
+  <si>
+    <t>router?</t>
   </si>
 </sst>
 </file>
@@ -574,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,24 +818,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988DF169-2626-45E6-A36A-F4AD1A4B6C9F}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600CCC3B-98C2-4D2B-BFEA-D00A9F2B4598}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -837,6 +866,26 @@
         <v>47</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Belegen in update-K. funktioniert jetzt, Problem lag im Backend, da .find verwendet wurde (gibt Array zurück), geändert zu .findOne
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9343F5-DC46-4D11-89AF-84C6A0D2F9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCC8D70-D3FD-4690-8264-D0300C0D0E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -190,12 +190,6 @@
     <t>await war wegen promise?</t>
   </si>
   <si>
-    <t>filter in Liste und Archiv funktionieren</t>
-  </si>
-  <si>
-    <t>in Liste bearbeiten und delte button bearbeitet</t>
-  </si>
-  <si>
     <t>reactive forms</t>
   </si>
   <si>
@@ -203,6 +197,18 @@
   </si>
   <si>
     <t>router?</t>
+  </si>
+  <si>
+    <t>formvontrolname vorne?</t>
+  </si>
+  <si>
+    <t>update Methode hinterlegen</t>
+  </si>
+  <si>
+    <t>create new erstellen!</t>
+  </si>
+  <si>
+    <t>FormGroup befüllen fixen! Weil es ein Array ist?</t>
   </si>
 </sst>
 </file>
@@ -590,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,23 +654,26 @@
       <c r="E6" t="s">
         <v>21</v>
       </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -732,7 +741,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E16" t="s">
@@ -740,7 +749,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
@@ -782,7 +791,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -809,6 +818,21 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -818,25 +842,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988DF169-2626-45E6-A36A-F4AD1A4B6C9F}">
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -845,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600CCC3B-98C2-4D2B-BFEA-D00A9F2B4598}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -873,17 +886,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update eines angelegten Tasks funktioniert (update-todo-K.)
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BB4056-2F3C-4B79-A20A-E3B92E3E4DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0409B6-375E-4C3A-9ABE-C91BCBE3C709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="30.09." sheetId="2" r:id="rId2"/>
+    <sheet name="03.10." sheetId="4" r:id="rId2"/>
     <sheet name="Notizen Präsi" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -163,21 +163,9 @@
     <t>dele one 30.09.</t>
   </si>
   <si>
-    <t>Backend starten</t>
-  </si>
-  <si>
-    <t>Frontend starten</t>
-  </si>
-  <si>
-    <t>klären === und == ?</t>
-  </si>
-  <si>
     <t>Archivbutton</t>
   </si>
   <si>
-    <t>await war wegen promise?</t>
-  </si>
-  <si>
     <t>reactive forms</t>
   </si>
   <si>
@@ -230,13 +218,196 @@
   </si>
   <si>
     <t>Frontend fertig gestalten  Header/Footer?</t>
+  </si>
+  <si>
+    <t>Nächste Schritte</t>
+  </si>
+  <si>
+    <t>update fertigstellen</t>
+  </si>
+  <si>
+    <t>delete mit Toast</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Prüfen, ob Input Felder ausgefüllt sind</t>
+  </si>
+  <si>
+    <t>Datenbank in MongoDb angelegt</t>
+  </si>
+  <si>
+    <t>== lockerer Vergleich, ggf. implizite Typkovertierung</t>
+  </si>
+  <si>
+    <t>=== strenger Vergleich (Wert und Typ) === verwenden!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warrtet bis Promise zurückgegeben wird, Funktion/Methode muss dann async </t>
+  </si>
+  <si>
+    <t>await war wegen promise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">klären === und == </t>
+  </si>
+  <si>
+    <t>Backend starten node --watch server.js</t>
+  </si>
+  <si>
+    <t>Frontend starten ng serve</t>
+  </si>
+  <si>
+    <t>Typescript und Javaskript</t>
+  </si>
+  <si>
+    <t>Formular wird in Tyescript angesprochen</t>
+  </si>
+  <si>
+    <t>Service aus Angular, um Parameter aus aktueller Route auszulesen</t>
+  </si>
+  <si>
+    <t>TS ist Obermenge von JS, TypeScript-Code wird compiliert und erzeugt JavaScript-Code, der vom Browser ausgeführt werden kann. 
+Im Gegensatz zu JavaScript ist TypeScript typsicher und klar objektorientiert</t>
+  </si>
+  <si>
+    <t>Fehlererkennung zur Kompilierzeit (früher)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Eine Komponente besteht aus einer </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>View</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Template</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) und einer TypeScript-Klasse. 
+Die AppComponent besteht z.B. aus der </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>app.component.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (der View) und der </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>app.component.ts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (der TypeScript-Klasse). 
+TypeScript-Klasse = Verwaltung der Daten, die in der View dargestellt und/oder durch Eingaben erzeugt werden (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logik</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> der Komponente)
+View ist der dargestellte Bereich der Komponente, also das, was man im Browser von der Komponente sieht.</t>
+    </r>
+  </si>
+  <si>
+    <t>Deployment (Frontend über github, Backend vercel oder render)</t>
+  </si>
+  <si>
+    <t>new umbenenn!</t>
+  </si>
+  <si>
+    <t>cancel click in update hinterlegt</t>
+  </si>
+  <si>
+    <t>Datepicker nach oben / unten begrenzen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +429,16 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +463,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -297,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -307,6 +492,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -641,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -653,9 +843,10 @@
     <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -663,7 +854,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
@@ -673,23 +864,32 @@
       <c r="F2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H2" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -697,29 +897,35 @@
       <c r="F5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -730,7 +936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -738,7 +944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -749,22 +955,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
@@ -773,17 +979,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
@@ -791,7 +997,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
         <v>30</v>
@@ -799,7 +1005,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
         <v>31</v>
@@ -811,6 +1017,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
@@ -819,11 +1028,17 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
       <c r="E21" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
       <c r="E22" t="s">
         <v>32</v>
       </c>
@@ -835,7 +1050,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -896,17 +1111,22 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -916,67 +1136,117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988DF169-2626-45E6-A36A-F4AD1A4B6C9F}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E9F4F2-232E-4CA2-88D6-731BA84F0CFF}">
+  <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600CCC3B-98C2-4D2B-BFEA-D00A9F2B4598}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="71.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+      <c r="B15" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modal bei Löschen funktioniert leider nicht
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0409B6-375E-4C3A-9ABE-C91BCBE3C709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DB51F3-F4C6-4B85-9387-6DCA27D1287D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -401,6 +401,12 @@
   </si>
   <si>
     <t>Datepicker nach oben / unten begrenzen</t>
+  </si>
+  <si>
+    <t>Modal!</t>
+  </si>
+  <si>
+    <t>Modal delete funktioniert nicht</t>
   </si>
 </sst>
 </file>
@@ -833,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -891,11 +897,11 @@
       <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s">
         <v>63</v>
@@ -905,7 +911,7 @@
       <c r="A6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H6" t="s">
@@ -1044,6 +1050,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Validator in Create-K. gesetzt
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E5B76F-AD85-49F4-A89C-8585BA38D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F90030-903A-4FAE-98B0-F86412739945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -118,12 +118,6 @@
     <t>Datum</t>
   </si>
   <si>
-    <t>Name + Datum</t>
-  </si>
-  <si>
-    <t>Datepicker keinen Text eingeben (darf kein Input Element sein?)</t>
-  </si>
-  <si>
     <t>Toast!</t>
   </si>
   <si>
@@ -145,12 +139,6 @@
     <t>Backend und Frontend verknüpfen</t>
   </si>
   <si>
-    <t xml:space="preserve">Deployment </t>
-  </si>
-  <si>
-    <t>JSON Dateiformat wdh (Infos im Body?)</t>
-  </si>
-  <si>
     <t>unterschied patch und put</t>
   </si>
   <si>
@@ -202,9 +190,6 @@
     <t>Abstand unter neues ToDo?</t>
   </si>
   <si>
-    <t>ist das doof, dass man das datum eingeben kann?</t>
-  </si>
-  <si>
     <t>noch zu erledigen</t>
   </si>
   <si>
@@ -214,28 +199,13 @@
     <t>abhaken --&gt; Task done und ins Archiv (Status muss geändert werden)</t>
   </si>
   <si>
-    <t>löschen Toast!</t>
-  </si>
-  <si>
     <t>Frontend fertig gestalten  Header/Footer?</t>
   </si>
   <si>
     <t>Nächste Schritte</t>
   </si>
   <si>
-    <t>update fertigstellen</t>
-  </si>
-  <si>
-    <t>delete mit Toast</t>
-  </si>
-  <si>
-    <t>create</t>
-  </si>
-  <si>
     <t>Deployment</t>
-  </si>
-  <si>
-    <t>Prüfen, ob Input Felder ausgefüllt sind</t>
   </si>
   <si>
     <t>Datenbank in MongoDb angelegt</t>
@@ -410,6 +380,21 @@
   </si>
   <si>
     <t>Toast oder und valid</t>
+  </si>
+  <si>
+    <t>create Toast!</t>
+  </si>
+  <si>
+    <t>create invalid/valid !!</t>
+  </si>
+  <si>
+    <t>create invalid!</t>
+  </si>
+  <si>
+    <t>delete Modal!</t>
+  </si>
+  <si>
+    <t>validator bei update</t>
   </si>
 </sst>
 </file>
@@ -840,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -870,11 +855,8 @@
       <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
       <c r="H2" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -882,46 +864,46 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H3" t="s">
-        <v>61</v>
+        <v>76</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -929,17 +911,17 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>20</v>
@@ -950,88 +932,77 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
       </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
+        <v>72</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>27</v>
+        <v>81</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>65</v>
-      </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
@@ -1040,32 +1011,23 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>80</v>
-      </c>
       <c r="E21" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" t="s">
-        <v>32</v>
+      <c r="E22" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" t="s">
-        <v>33</v>
+      <c r="E23" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1091,7 +1053,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1099,7 +1061,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
@@ -1107,7 +1069,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
@@ -1126,22 +1088,37 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1139,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1172,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600CCC3B-98C2-4D2B-BFEA-D00A9F2B4598}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1186,59 +1163,59 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1248,20 +1225,25 @@
     </row>
     <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
-        <v>79</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
markAsDone in List erstellt
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F90030-903A-4FAE-98B0-F86412739945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A73DE0-B47B-4677-A05A-E1B5816501AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>validator bei update</t>
+  </si>
+  <si>
+    <t>Promises richtig verstehen Promisekette?</t>
   </si>
 </sst>
 </file>
@@ -827,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1149,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600CCC3B-98C2-4D2B-BFEA-D00A9F2B4598}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1246,6 +1249,11 @@
         <v>33</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Angular Material installiert, Modal Dialog funktioniert noch nicht beim Löschen
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A73DE0-B47B-4677-A05A-E1B5816501AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F220C60C-DBAD-48F3-AC90-85131A5A1DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Listenansicht Sortierung nach Datum</t>
-  </si>
-  <si>
-    <t>bearbeiten</t>
   </si>
   <si>
     <t>Komponenten</t>
@@ -397,7 +394,16 @@
     <t>validator bei update</t>
   </si>
   <si>
-    <t>Promises richtig verstehen Promisekette?</t>
+    <t>Promises richtig verstehen Promisekette? Muss immer return, damit then funktioniert?</t>
+  </si>
+  <si>
+    <t>Archiv einrichtenb!</t>
+  </si>
+  <si>
+    <t>bei anlage buttons noch klein</t>
+  </si>
+  <si>
+    <t>Suchleiste</t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -494,6 +500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -828,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -848,161 +855,155 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H2" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
+        <v>49</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>80</v>
+        <v>18</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>69</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
+        <v>47</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E12" t="s">
-        <v>44</v>
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="1" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>72</v>
-      </c>
       <c r="E17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E18" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1010,27 +1011,27 @@
         <v>10</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E21" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1056,7 +1057,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1064,7 +1065,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
@@ -1072,7 +1073,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
@@ -1091,37 +1092,57 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1142,7 +1163,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1154,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600CCC3B-98C2-4D2B-BFEA-D00A9F2B4598}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1166,59 +1187,59 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1228,30 +1249,30 @@
     </row>
     <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modal Dialog funktioniert nicht, als Alternative jetzt window.confirm eingefügt
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F220C60C-DBAD-48F3-AC90-85131A5A1DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AE9163-5603-4F1F-BD5B-34600A8FBA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -376,9 +376,6 @@
     <t>create läuft</t>
   </si>
   <si>
-    <t>Toast oder und valid</t>
-  </si>
-  <si>
     <t>create Toast!</t>
   </si>
   <si>
@@ -404,6 +401,12 @@
   </si>
   <si>
     <t>Suchleiste</t>
+  </si>
+  <si>
+    <t>modal dialog in angular mit datenübergabe</t>
+  </si>
+  <si>
+    <t>Toast</t>
   </si>
 </sst>
 </file>
@@ -837,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -874,7 +877,7 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -887,7 +890,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>17</v>
@@ -896,7 +899,7 @@
         <v>72</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -907,7 +910,7 @@
         <v>18</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -923,7 +926,7 @@
         <v>69</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -959,7 +962,7 @@
         <v>25</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -972,12 +975,15 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="H13" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>15</v>
@@ -1122,7 +1128,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1132,7 +1138,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -1272,7 +1278,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suchzeile in List funktioniert
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AE9163-5603-4F1F-BD5B-34600A8FBA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A234DA-B71D-44A3-B97B-0A3DA1C4FF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -407,6 +407,12 @@
   </si>
   <si>
     <t>Toast</t>
+  </si>
+  <si>
+    <t>was sagt mir das hier: private router = inject(Router);</t>
+  </si>
+  <si>
+    <t>Strings einheitlich</t>
   </si>
 </sst>
 </file>
@@ -840,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -879,6 +885,9 @@
       <c r="F3" t="s">
         <v>85</v>
       </c>
+      <c r="H3" s="10" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -910,7 +919,7 @@
         <v>18</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -920,14 +929,14 @@
       <c r="E7" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="H7" s="10" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -961,9 +970,6 @@
       <c r="F11" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -993,6 +999,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1179,7 +1188,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600CCC3B-98C2-4D2B-BFEA-D00A9F2B4598}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
@@ -1281,6 +1290,11 @@
         <v>80</v>
       </c>
     </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Erledigte Komponenten aktualisiert, Suchzeile ergänzt
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A234DA-B71D-44A3-B97B-0A3DA1C4FF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE519EB-E75B-412A-8A50-7277EFD4B436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
   <si>
     <t>To Dos App PCT</t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>Strings einheitlich</t>
+  </si>
+  <si>
+    <t>Link muss hinter button nicht icon liegen!</t>
+  </si>
+  <si>
+    <t>invalid update</t>
   </si>
 </sst>
 </file>
@@ -846,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -978,6 +984,9 @@
       <c r="E12" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="H12" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1012,6 +1021,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Links müssen in Button liegen, nicht in Icon-Tag
</commit_message>
<xml_diff>
--- a/To Dos#.xlsx
+++ b/To Dos#.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadja\Documents\PCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE519EB-E75B-412A-8A50-7277EFD4B436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56480823-789D-47C4-81E5-24F325551FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1660FCD3-2F36-42FA-BEA4-C05A7BB702D2}"/>
   </bookViews>
@@ -850,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DE875-1081-4EEB-883D-6875951373BC}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -924,9 +924,6 @@
       <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1021,9 +1018,6 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>88</v>
-      </c>
       <c r="E17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1170,6 +1164,16 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>